<commit_message>
components finished. need to add individual componentData tables now
</commit_message>
<xml_diff>
--- a/notes/ECS_Design.xlsx
+++ b/notes/ECS_Design.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\AdventureGame_MUD_ECS\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\code\adv\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEE86DD-1989-451B-A4A2-4F9BF6B09912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="2190" windowWidth="18750" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
     <sheet name="Components" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>Item</t>
   </si>
@@ -61,9 +60,6 @@
     <t>Entities</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -112,9 +108,6 @@
     <t>Response</t>
   </si>
   <si>
-    <t>ResponseText</t>
-  </si>
-  <si>
     <t>Spell</t>
   </si>
   <si>
@@ -151,9 +144,6 @@
     <t>Agility</t>
   </si>
   <si>
-    <t>Intellect</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -163,12 +153,6 @@
     <t>[]</t>
   </si>
   <si>
-    <t>LocationType</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>ContainerList</t>
   </si>
   <si>
@@ -208,18 +192,12 @@
     <t>DispositionList</t>
   </si>
   <si>
-    <t>DispositionTag</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>DispositionTagId</t>
   </si>
   <si>
-    <t>DispositionStatus</t>
-  </si>
-  <si>
     <t>DispositionValue</t>
   </si>
   <si>
@@ -254,12 +232,84 @@
   </si>
   <si>
     <t>GlobalConditionList</t>
+  </si>
+  <si>
+    <t>StrengthModifier</t>
+  </si>
+  <si>
+    <t>AgilityModifier</t>
+  </si>
+  <si>
+    <t>IntelligenceModifier</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
+  </si>
+  <si>
+    <t>NaturalDamage</t>
+  </si>
+  <si>
+    <t>EquipSlot</t>
+  </si>
+  <si>
+    <t>Head</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Arms</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Main Hand</t>
+  </si>
+  <si>
+    <t>Off Hand</t>
+  </si>
+  <si>
+    <t>Trinket</t>
+  </si>
+  <si>
+    <t>EquipSlot types: head, chest, arms, legs, main hand, off hand, trinket</t>
+  </si>
+  <si>
+    <t>ListPriority</t>
+  </si>
+  <si>
+    <t>WhereText</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>ContainerSlot</t>
+  </si>
+  <si>
+    <t>ItemId</t>
+  </si>
+  <si>
+    <t>IsInInventory</t>
+  </si>
+  <si>
+    <t>DropsOnDeath</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>CategoryList</t>
+  </si>
+  <si>
+    <t>EquipSlots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -331,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,13 +410,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -648,12 +701,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D24" sqref="D24"/>
+      <selection pane="topRight" activeCell="S2" sqref="S2:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,33 +714,32 @@
     <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="8" t="s">
         <v>1</v>
@@ -696,10 +748,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>13</v>
@@ -711,242 +763,224 @@
         <v>15</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="P2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="J11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>27</v>
+      <c r="M13" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="W15" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>33</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -956,12 +990,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,9 +1003,9 @@
     <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
@@ -984,8 +1018,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>36</v>
+      <c r="A1" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -997,8 +1031,8 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1006,7 +1040,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1031,16 +1065,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1048,7 +1082,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>3</v>
@@ -1056,73 +1090,91 @@
     </row>
     <row r="5" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1130,211 +1182,250 @@
         <v>21</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="7" t="s">
+    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="F23" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="7" t="s">
+    </row>
+    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>42</v>
+      <c r="C28" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Active to GlobalCondition
</commit_message>
<xml_diff>
--- a/notes/ECS_Design.xlsx
+++ b/notes/ECS_Design.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\code\adv\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\AdventureGame_MUD_ECS\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280418F8-AA88-484F-B5E9-270DBE171795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="5460" yWindow="3300" windowWidth="21465" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -20,18 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="92">
   <si>
     <t>Item</t>
   </si>
@@ -304,12 +299,15 @@
   </si>
   <si>
     <t>EquipSlots</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,14 +411,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,7 +699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -990,12 +988,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D19" sqref="D19"/>
+      <selection pane="topRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1016,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="3"/>
@@ -1031,8 +1029,8 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1040,7 +1038,7 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1173,7 +1171,7 @@
       <c r="C11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1364,6 +1362,9 @@
       </c>
       <c r="D25" s="6" t="s">
         <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
did things. Disposition added as foreign key component data example
</commit_message>
<xml_diff>
--- a/notes/ECS_Design.xlsx
+++ b/notes/ECS_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\AdventureGame_MUD_ECS\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280418F8-AA88-484F-B5E9-270DBE171795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872AF505-CF34-46C4-B9B4-64A9B504E9A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="3300" windowWidth="21465" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="1365" windowWidth="21465" windowHeight="15150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>DispositionTagId</t>
-  </si>
-  <si>
     <t>DispositionValue</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>CategoryTagId</t>
   </si>
 </sst>
 </file>
@@ -797,10 +797,10 @@
         <v>43</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -993,7 +993,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E25" sqref="E25"/>
+      <selection pane="topRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,10 +1069,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>3</v>
@@ -1097,10 +1097,10 @@
         <v>36</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
     </row>
     <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>39</v>
@@ -1146,16 +1146,16 @@
         <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="13"/>
@@ -1166,13 +1166,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1257,16 +1257,16 @@
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>44</v>
@@ -1307,15 +1307,15 @@
         <v>14</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>44</v>
@@ -1364,12 +1364,12 @@
         <v>1</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>39</v>
@@ -1380,47 +1380,47 @@
         <v>12</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="F28" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial commit Response List and updated Excel
</commit_message>
<xml_diff>
--- a/notes/ECS_Design.xlsx
+++ b/notes/ECS_Design.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
     <sheet name="Components" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -335,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +360,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -373,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,11 +420,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -686,7 +713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,7 +1014,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1052,373 +1079,262 @@
       <c r="R2" s="11"/>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="1:19" s="6" customFormat="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:19" s="19" customFormat="1">
+      <c r="A3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:19" s="19" customFormat="1">
+      <c r="A4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" s="6" customFormat="1">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="5" spans="1:19" s="19" customFormat="1">
+      <c r="A5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:19" s="19" customFormat="1">
+      <c r="A6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" s="6" customFormat="1">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="7" spans="1:19" s="19" customFormat="1">
+      <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-    </row>
-    <row r="8" spans="1:19" s="7" customFormat="1">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:19" s="19" customFormat="1">
+      <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="6" customFormat="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:19" s="19" customFormat="1">
+      <c r="A9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+    </row>
+    <row r="11" spans="1:19" s="19" customFormat="1">
+      <c r="A11" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="7" customFormat="1">
+      <c r="A12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+    </row>
+    <row r="13" spans="1:19" s="19" customFormat="1">
+      <c r="A13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="19" customFormat="1">
+      <c r="A14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" s="6" customFormat="1">
+      <c r="A15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+    </row>
+    <row r="16" spans="1:19" s="7" customFormat="1">
+      <c r="A16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+    </row>
+    <row r="17" spans="1:19" s="19" customFormat="1">
+      <c r="A17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" s="19" customFormat="1">
+      <c r="A18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" s="6" customFormat="1">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="7" customFormat="1">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" s="6" customFormat="1">
-      <c r="A13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-    </row>
-    <row r="14" spans="1:19" s="7" customFormat="1">
-      <c r="A14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" s="6" customFormat="1">
-      <c r="A15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-    </row>
-    <row r="16" spans="1:19" s="7" customFormat="1">
-      <c r="A16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="1:19" s="6" customFormat="1">
-      <c r="A17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" s="7" customFormat="1">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1436,120 +1352,118 @@
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
     </row>
-    <row r="19" spans="1:19" s="6" customFormat="1">
-      <c r="A19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>50</v>
+    <row r="19" spans="1:19" s="7" customFormat="1">
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="7" customFormat="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" s="6" customFormat="1">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="7" customFormat="1">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="6" customFormat="1">
-      <c r="A21" s="5" t="s">
+    <row r="23" spans="1:19" s="6" customFormat="1">
+      <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" s="7" customFormat="1">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" s="6" customFormat="1">
-      <c r="A23" s="4" t="s">
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+    </row>
+    <row r="24" spans="1:19" s="19" customFormat="1">
+      <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" s="7" customFormat="1">
-      <c r="A24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1564,92 +1478,104 @@
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
     </row>
-    <row r="25" spans="1:19" s="6" customFormat="1">
+    <row r="25" spans="1:19" s="7" customFormat="1">
       <c r="A25" s="5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-    </row>
-    <row r="26" spans="1:19" s="7" customFormat="1">
+        <v>81</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:19" s="6" customFormat="1">
       <c r="A26" s="5" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:19" s="6" customFormat="1">
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+    </row>
+    <row r="27" spans="1:19" s="7" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-    </row>
-    <row r="28" spans="1:19" s="7" customFormat="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="19" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>3</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
     </row>
     <row r="29" spans="1:19">
       <c r="B29" t="s">
@@ -1658,7 +1584,7 @@
     </row>
   </sheetData>
   <sortState ref="A3:S29">
-    <sortCondition ref="A3:A29"/>
+    <sortCondition sortBy="cellColor" ref="A3:A29" dxfId="1"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="L1:M1"/>

</xml_diff>